<commit_message>
including IssuerCreditOpinions Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Financial_AuditTrial_Data.xlsx
+++ b/src/test/resources/Financial_AuditTrial_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="131">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>FC_TANGIBLE_COMMON_EQUITY_TANGIBLE_ASSETS_BNK</t>
-  </si>
-  <si>
-    <t>FC_NET_INCOME_MINUS_CASH_DIV_TOTAL_EQUITY_BNK</t>
   </si>
   <si>
     <t>FC_NPL_GROSS_LOANS_BNK</t>
@@ -786,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:XFD122"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +816,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +832,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +864,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +880,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +888,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -907,7 +904,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,7 +912,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -923,7 +920,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +936,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,7 +944,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,7 +952,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,7 +960,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,7 +968,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +976,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +984,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +992,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +1000,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1011,7 +1008,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1016,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,7 +1024,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1032,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,7 +1040,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,7 +1048,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,7 +1056,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,7 +1064,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1075,7 +1072,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1083,7 +1080,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1091,7 +1088,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,7 +1096,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1107,7 +1104,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1115,7 +1112,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1120,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,7 +1128,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,7 +1136,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1144,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1155,7 +1152,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1163,7 +1160,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1171,7 +1168,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1179,7 +1176,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1187,7 +1184,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,7 +1192,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,7 +1200,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1211,7 +1208,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1216,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1227,7 +1224,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,7 +1232,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1243,7 +1240,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,7 +1248,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1259,7 +1256,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1264,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,7 +1272,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1283,7 +1280,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1288,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1299,7 +1296,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1307,7 +1304,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1315,7 +1312,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,7 +1320,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1331,7 +1328,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1339,7 +1336,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1347,7 +1344,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1355,7 +1352,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1363,7 +1360,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1368,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1379,7 +1376,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1387,7 +1384,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1392,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1403,7 +1400,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1411,7 +1408,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1419,7 +1416,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1427,7 +1424,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1432,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1440,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1448,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1456,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1464,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1475,7 +1472,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1480,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1488,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1496,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1504,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,7 +1512,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,7 +1520,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1531,7 +1528,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,7 +1536,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1547,7 +1544,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,7 +1552,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1560,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1568,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1576,7 @@
         <v>98</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1587,7 +1584,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1595,7 +1592,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1603,7 +1600,7 @@
         <v>101</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,7 +1608,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1616,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,7 +1624,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,7 +1632,7 @@
         <v>105</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1640,7 @@
         <v>106</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1648,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1659,7 +1656,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1667,7 +1664,7 @@
         <v>109</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1675,7 +1672,7 @@
         <v>110</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1683,7 +1680,7 @@
         <v>111</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1691,7 +1688,7 @@
         <v>112</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1699,7 +1696,7 @@
         <v>113</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1707,7 +1704,7 @@
         <v>114</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1715,7 +1712,7 @@
         <v>115</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -1723,7 +1720,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1728,7 @@
         <v>117</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1739,7 +1736,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -1747,7 +1744,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1755,7 +1752,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1763,7 +1760,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1771,7 +1768,7 @@
         <v>122</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -1779,7 +1776,7 @@
         <v>123</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1787,7 +1784,7 @@
         <v>124</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1795,7 +1792,7 @@
         <v>125</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1803,7 +1800,7 @@
         <v>126</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -1811,7 +1808,7 @@
         <v>127</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -1819,7 +1816,7 @@
         <v>128</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1827,23 +1824,15 @@
         <v>129</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A130">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A1:A129">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>IF(FIND(" ",$A1)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>